<commit_message>
Unsaved changes to Module 1 quiz 1
</commit_message>
<xml_diff>
--- a/Module1/Lab1Start v5 RW.xlsx
+++ b/Module1/Lab1Start v5 RW.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ahath\OneDrive\Documents\RW\Excel_study\Excel_files_workspace\Excel courses\edX Introduction to Data Analysis using Excel\course_repo\Module1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A23EF30-69B2-431C-B05C-FC8EB01E1953}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71853DF6-0381-4916-959A-2A7A7DEED304}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12334" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -125,14 +125,14 @@
   </cellStyleXfs>
   <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -591,6 +591,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000001-957E-4A38-95C9-5AEBB72CBB36}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="1"/>
@@ -606,6 +611,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000003-957E-4A38-95C9-5AEBB72CBB36}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="2"/>
@@ -621,6 +631,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000005-957E-4A38-95C9-5AEBB72CBB36}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:cat>
             <c:strRef>
@@ -799,7 +814,7 @@
       <c:layout/>
       <c:barChart>
         <c:barDir val="col"/>
-        <c:grouping val="stacked"/>
+        <c:grouping val="clustered"/>
         <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
@@ -1068,7 +1083,6 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:overlap val="100"/>
         <c:axId val="712375840"/>
         <c:axId val="655989728"/>
       </c:barChart>
@@ -1759,6 +1773,7 @@
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:crossAx val="572816384"/>
+        <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
@@ -4480,8 +4495,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:P9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="R23" sqref="R23"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="F27" sqref="F27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -4496,28 +4511,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:16" x14ac:dyDescent="0.4">
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1"/>
+      <c r="C1" s="4"/>
+      <c r="D1" s="4"/>
+      <c r="E1" s="4"/>
+      <c r="F1" s="4"/>
+      <c r="G1" s="4"/>
+      <c r="H1" s="4"/>
     </row>
     <row r="2" spans="2:16" x14ac:dyDescent="0.4">
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
-      <c r="G2" s="2"/>
-      <c r="H2" s="2"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
+      <c r="F2" s="3"/>
+      <c r="G2" s="3"/>
+      <c r="H2" s="3"/>
     </row>
     <row r="3" spans="2:16" x14ac:dyDescent="0.4">
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="1" t="s">
         <v>10</v>
       </c>
       <c r="C3">
@@ -4549,30 +4564,30 @@
       <c r="B4" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="4"/>
-      <c r="D4" s="4"/>
-      <c r="E4" s="4">
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2">
         <v>3384215</v>
       </c>
-      <c r="F4" s="4">
+      <c r="F4" s="2">
         <v>4293592</v>
       </c>
-      <c r="G4" s="4">
+      <c r="G4" s="2">
         <v>3285954</v>
       </c>
-      <c r="H4" s="4">
+      <c r="H4" s="2">
         <v>4154231</v>
       </c>
       <c r="K4" t="s">
         <v>3</v>
       </c>
-      <c r="L4" s="4">
+      <c r="L4" s="2">
         <v>21302059</v>
       </c>
       <c r="O4" t="s">
         <v>2</v>
       </c>
-      <c r="P4" s="4">
+      <c r="P4" s="2">
         <v>15117992</v>
       </c>
     </row>
@@ -4580,34 +4595,34 @@
       <c r="B5" t="s">
         <v>9</v>
       </c>
-      <c r="C5" s="4">
+      <c r="C5" s="2">
         <v>8964888</v>
       </c>
-      <c r="D5" s="4">
+      <c r="D5" s="2">
         <v>9175983</v>
       </c>
-      <c r="E5" s="4">
+      <c r="E5" s="2">
         <v>9858787</v>
       </c>
-      <c r="F5" s="4">
+      <c r="F5" s="2">
         <v>7611243</v>
       </c>
-      <c r="G5" s="4">
+      <c r="G5" s="2">
         <v>14799083</v>
       </c>
-      <c r="H5" s="4">
+      <c r="H5" s="2">
         <v>11372150</v>
       </c>
       <c r="K5" t="s">
         <v>1</v>
       </c>
-      <c r="L5" s="4">
+      <c r="L5" s="2">
         <v>7935738</v>
       </c>
       <c r="O5" t="s">
         <v>9</v>
       </c>
-      <c r="P5" s="4">
+      <c r="P5" s="2">
         <v>61782134</v>
       </c>
     </row>
@@ -4615,30 +4630,30 @@
       <c r="B6" t="s">
         <v>8</v>
       </c>
-      <c r="C6" s="4"/>
-      <c r="D6" s="4"/>
-      <c r="E6" s="4">
+      <c r="C6" s="2"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2">
         <v>1997035</v>
       </c>
-      <c r="F6" s="4">
+      <c r="F6" s="2">
         <v>2247889</v>
       </c>
-      <c r="G6" s="4">
+      <c r="G6" s="2">
         <v>1938954</v>
       </c>
-      <c r="H6" s="4">
+      <c r="H6" s="2">
         <v>2187004</v>
       </c>
       <c r="K6" t="s">
         <v>6</v>
       </c>
-      <c r="L6" s="4">
+      <c r="L6" s="2">
         <v>8432872</v>
       </c>
       <c r="O6" t="s">
         <v>8</v>
       </c>
-      <c r="P6" s="4">
+      <c r="P6" s="2">
         <v>8370882</v>
       </c>
     </row>
@@ -4646,7 +4661,7 @@
       <c r="K7" t="s">
         <v>5</v>
       </c>
-      <c r="L7" s="4">
+      <c r="L7" s="2">
         <v>8978596</v>
       </c>
     </row>
@@ -4654,7 +4669,7 @@
       <c r="K8" t="s">
         <v>7</v>
       </c>
-      <c r="L8" s="4">
+      <c r="L8" s="2">
         <v>10646196</v>
       </c>
     </row>
@@ -4662,7 +4677,7 @@
       <c r="K9" t="s">
         <v>4</v>
       </c>
-      <c r="L9" s="4">
+      <c r="L9" s="2">
         <v>27975547</v>
       </c>
     </row>

</xml_diff>